<commit_message>
DONALD-2 Correction of the variables according to today's discussion. Only the operation for education and the variable for dietary assessment are missing.
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_DONALD_P1.xlsx
+++ b/rmonize/data_dictionary/DD_DONALD_P1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="282">
   <si>
     <t>index</t>
   </si>
@@ -49,9 +49,6 @@
     <t>sex</t>
   </si>
   <si>
-    <t>EDU_LEVEL_P</t>
-  </si>
-  <si>
     <t>TOT_PA_QX</t>
   </si>
   <si>
@@ -781,9 +778,6 @@
     <t>Physical activity from questionnaire data [MET-hr/week]</t>
   </si>
   <si>
-    <t>parental education status</t>
-  </si>
-  <si>
     <t>Age [years] at dietary assessment (1. record day)</t>
   </si>
   <si>
@@ -796,36 +790,6 @@
     <t>integer</t>
   </si>
   <si>
-    <t>Early Childhood Education</t>
-  </si>
-  <si>
-    <t>Primary Education</t>
-  </si>
-  <si>
-    <t>Lower Secondary Education</t>
-  </si>
-  <si>
-    <t>Upper Secondary Education</t>
-  </si>
-  <si>
-    <t>Post-secondary non-tertiary education</t>
-  </si>
-  <si>
-    <t>Short-Cycle Tertiary Education</t>
-  </si>
-  <si>
-    <t>Bachelor's or equivalent level</t>
-  </si>
-  <si>
-    <t>Master's or equivalent level</t>
-  </si>
-  <si>
-    <t>Doctoral or equivalent level</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Smoker in Household [yes/no]</t>
   </si>
   <si>
@@ -836,6 +800,72 @@
   </si>
   <si>
     <t>Geschlecht</t>
+  </si>
+  <si>
+    <t>m_schulab</t>
+  </si>
+  <si>
+    <t>v_schulab</t>
+  </si>
+  <si>
+    <t>b_berufsab</t>
+  </si>
+  <si>
+    <t>v_berufsab</t>
+  </si>
+  <si>
+    <t>Schuldbildung der Mutter</t>
+  </si>
+  <si>
+    <t>Schuldbildung des Vaters</t>
+  </si>
+  <si>
+    <t>Berufsabschluss der Mutter</t>
+  </si>
+  <si>
+    <t>Berufsabschluss des Vaters</t>
+  </si>
+  <si>
+    <t>Volks-/Hauptschulabschluss</t>
+  </si>
+  <si>
+    <t>Mittlere Reife, Realschulabschluss (Fachschulreife)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fachhochschulreife, Abschluss einer Fachoberschule etc.       </t>
+  </si>
+  <si>
+    <t>Abitur (Hochschulreife)</t>
+  </si>
+  <si>
+    <t>keinen dieser Abschlüsse</t>
+  </si>
+  <si>
+    <t>m_berufsab</t>
+  </si>
+  <si>
+    <t>Lehre (beruflich-betriebliche Ausbildung)</t>
+  </si>
+  <si>
+    <t>Berufsschule, Handelsschule (berufl.-schulische Ausbildung)</t>
+  </si>
+  <si>
+    <t>Fachschule (z.B. Meister-Technikerschule, Berufs/Fachakademie)</t>
+  </si>
+  <si>
+    <t>Fachhochschule, Ingenieurschule</t>
+  </si>
+  <si>
+    <t>Universität, Hochschule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anderer Abschluss (bis 3/2016 berufl. Praktikum)                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kein beruflicher Abschluss     </t>
+  </si>
+  <si>
+    <t>noch in beruflicher Ausbildung (Auszubildener / Student)</t>
   </si>
 </sst>
 </file>
@@ -1174,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1212,7 +1242,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1223,10 +1253,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1237,7 +1267,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -1248,13 +1278,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>260</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="D5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1262,13 +1292,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>261</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1276,13 +1306,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>262</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1290,13 +1320,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>263</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>132</v>
+        <v>267</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -1304,10 +1334,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>133</v>
+        <v>251</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1318,13 +1348,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>134</v>
+        <v>256</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1332,10 +1362,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -1346,10 +1376,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -1360,10 +1390,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -1374,10 +1404,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -1388,10 +1418,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -1402,10 +1432,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -1416,10 +1446,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -1430,10 +1460,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -1444,10 +1474,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -1458,10 +1488,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
@@ -1472,10 +1502,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -1486,10 +1516,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
@@ -1500,10 +1530,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -1514,10 +1544,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
@@ -1528,10 +1558,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
@@ -1542,10 +1572,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -1556,10 +1586,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -1570,10 +1600,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
@@ -1584,10 +1614,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -1598,10 +1628,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
@@ -1612,10 +1642,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
@@ -1626,10 +1656,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D32" t="s">
         <v>5</v>
@@ -1640,10 +1670,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -1654,10 +1684,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
@@ -1668,10 +1698,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -1682,10 +1712,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
@@ -1696,10 +1726,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D37" t="s">
         <v>5</v>
@@ -1710,10 +1740,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D38" t="s">
         <v>5</v>
@@ -1724,10 +1754,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
@@ -1738,10 +1768,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
@@ -1752,10 +1782,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D41" t="s">
         <v>5</v>
@@ -1766,10 +1796,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D42" t="s">
         <v>5</v>
@@ -1780,10 +1810,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D43" t="s">
         <v>5</v>
@@ -1794,10 +1824,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
@@ -1808,10 +1838,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
@@ -1822,10 +1852,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
@@ -1836,10 +1866,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D47" t="s">
         <v>5</v>
@@ -1850,10 +1880,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D48" t="s">
         <v>5</v>
@@ -1864,10 +1894,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
@@ -1878,10 +1908,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D50" t="s">
         <v>5</v>
@@ -1892,10 +1922,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
         <v>5</v>
@@ -1906,10 +1936,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D52" t="s">
         <v>5</v>
@@ -1920,10 +1950,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D53" t="s">
         <v>5</v>
@@ -1934,10 +1964,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D54" t="s">
         <v>5</v>
@@ -1948,10 +1978,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D55" t="s">
         <v>5</v>
@@ -1962,10 +1992,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
@@ -1976,10 +2006,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D57" t="s">
         <v>5</v>
@@ -1990,10 +2020,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D58" t="s">
         <v>5</v>
@@ -2004,10 +2034,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D59" t="s">
         <v>5</v>
@@ -2018,10 +2048,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D60" t="s">
         <v>5</v>
@@ -2032,10 +2062,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D61" t="s">
         <v>5</v>
@@ -2046,10 +2076,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D62" t="s">
         <v>5</v>
@@ -2060,10 +2090,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D63" t="s">
         <v>5</v>
@@ -2074,10 +2104,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D64" t="s">
         <v>5</v>
@@ -2088,10 +2118,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D65" t="s">
         <v>5</v>
@@ -2102,10 +2132,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D66" t="s">
         <v>5</v>
@@ -2116,10 +2146,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D67" t="s">
         <v>5</v>
@@ -2130,10 +2160,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D68" t="s">
         <v>5</v>
@@ -2144,10 +2174,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D69" t="s">
         <v>5</v>
@@ -2158,10 +2188,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D70" t="s">
         <v>5</v>
@@ -2172,10 +2202,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D71" t="s">
         <v>5</v>
@@ -2186,10 +2216,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D72" t="s">
         <v>5</v>
@@ -2200,10 +2230,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D73" t="s">
         <v>5</v>
@@ -2214,10 +2244,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D74" t="s">
         <v>5</v>
@@ -2228,10 +2258,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D75" t="s">
         <v>5</v>
@@ -2242,10 +2272,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D76" t="s">
         <v>5</v>
@@ -2256,10 +2286,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D77" t="s">
         <v>5</v>
@@ -2270,10 +2300,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D78" t="s">
         <v>5</v>
@@ -2284,10 +2314,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D79" t="s">
         <v>5</v>
@@ -2298,10 +2328,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D80" t="s">
         <v>5</v>
@@ -2312,10 +2342,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D81" t="s">
         <v>5</v>
@@ -2326,10 +2356,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D82" t="s">
         <v>5</v>
@@ -2340,10 +2370,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D83" t="s">
         <v>5</v>
@@ -2354,10 +2384,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D84" t="s">
         <v>5</v>
@@ -2368,10 +2398,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D85" t="s">
         <v>5</v>
@@ -2382,10 +2412,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D86" t="s">
         <v>5</v>
@@ -2396,10 +2426,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D87" t="s">
         <v>5</v>
@@ -2410,10 +2440,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D88" t="s">
         <v>5</v>
@@ -2424,10 +2454,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D89" t="s">
         <v>5</v>
@@ -2438,10 +2468,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D90" t="s">
         <v>5</v>
@@ -2452,10 +2482,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D91" t="s">
         <v>5</v>
@@ -2466,10 +2496,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D92" t="s">
         <v>5</v>
@@ -2480,10 +2510,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D93" t="s">
         <v>5</v>
@@ -2494,10 +2524,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D94" t="s">
         <v>5</v>
@@ -2508,10 +2538,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D95" t="s">
         <v>5</v>
@@ -2522,10 +2552,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D96" t="s">
         <v>5</v>
@@ -2536,10 +2566,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D97" t="s">
         <v>5</v>
@@ -2550,10 +2580,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D98" t="s">
         <v>5</v>
@@ -2564,10 +2594,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D99" t="s">
         <v>5</v>
@@ -2578,10 +2608,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D100" t="s">
         <v>5</v>
@@ -2592,10 +2622,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D101" t="s">
         <v>5</v>
@@ -2606,10 +2636,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D102" t="s">
         <v>5</v>
@@ -2620,10 +2650,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D103" t="s">
         <v>5</v>
@@ -2634,10 +2664,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D104" t="s">
         <v>5</v>
@@ -2648,10 +2678,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D105" t="s">
         <v>5</v>
@@ -2662,10 +2692,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D106" t="s">
         <v>5</v>
@@ -2676,10 +2706,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D107" t="s">
         <v>5</v>
@@ -2690,10 +2720,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D108" t="s">
         <v>5</v>
@@ -2704,10 +2734,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D109" t="s">
         <v>5</v>
@@ -2718,10 +2748,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D110" t="s">
         <v>5</v>
@@ -2732,10 +2762,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D111" t="s">
         <v>5</v>
@@ -2746,10 +2776,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D112" t="s">
         <v>5</v>
@@ -2760,10 +2790,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D113" t="s">
         <v>5</v>
@@ -2774,10 +2804,10 @@
         <v>113</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D114" t="s">
         <v>5</v>
@@ -2788,10 +2818,10 @@
         <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D115" t="s">
         <v>5</v>
@@ -2802,10 +2832,10 @@
         <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D116" t="s">
         <v>5</v>
@@ -2816,10 +2846,10 @@
         <v>116</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D117" t="s">
         <v>5</v>
@@ -2830,10 +2860,10 @@
         <v>117</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D118" t="s">
         <v>5</v>
@@ -2844,10 +2874,10 @@
         <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D119" t="s">
         <v>5</v>
@@ -2858,10 +2888,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D120" t="s">
         <v>5</v>
@@ -2872,10 +2902,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D121" t="s">
         <v>5</v>
@@ -2886,10 +2916,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D122" t="s">
         <v>5</v>
@@ -2900,10 +2930,10 @@
         <v>122</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D123" t="s">
         <v>5</v>
@@ -2914,10 +2944,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D124" t="s">
         <v>5</v>
@@ -2928,10 +2958,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D125" t="s">
         <v>5</v>
@@ -2942,10 +2972,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D126" t="s">
         <v>5</v>
@@ -2956,12 +2986,54 @@
         <v>126</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D130" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2973,10 +3045,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3004,7 +3076,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -3015,139 +3087,315 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>260</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>260</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>260</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>260</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>260</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>261</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>261</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>261</v>
       </c>
       <c r="B11">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>261</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>261</v>
       </c>
       <c r="B13">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>273</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>11</v>
+        <v>273</v>
       </c>
       <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B22">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
-        <v>270</v>
+      <c r="C22" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DONALD-4 all files for P1 and P2
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_DONALD_P1.xlsx
+++ b/rmonize/data_dictionary/DD_DONALD_P1.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E2CDD8-DCB9-4A5F-866A-B5B1214CAEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="281">
   <si>
     <t>index</t>
   </si>
@@ -808,12 +809,6 @@
     <t>v_schulab</t>
   </si>
   <si>
-    <t>b_berufsab</t>
-  </si>
-  <si>
-    <t>v_berufsab</t>
-  </si>
-  <si>
     <t>Schuldbildung der Mutter</t>
   </si>
   <si>
@@ -841,9 +836,6 @@
     <t>keinen dieser Abschlüsse</t>
   </si>
   <si>
-    <t>m_berufsab</t>
-  </si>
-  <si>
     <t>Lehre (beruflich-betriebliche Ausbildung)</t>
   </si>
   <si>
@@ -866,12 +858,18 @@
   </si>
   <si>
     <t>noch in beruflicher Ausbildung (Auszubildener / Student)</t>
+  </si>
+  <si>
+    <t>m_berufab</t>
+  </si>
+  <si>
+    <t>v_berufab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -926,7 +924,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1203,21 +1201,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A130"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.54296875" customWidth="1"/>
-    <col min="3" max="3" width="55.26953125" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1231,7 +1229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1245,7 +1243,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1259,7 +1257,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1273,7 +1271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1281,13 +1279,13 @@
         <v>260</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D5" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1295,41 +1293,41 @@
         <v>261</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D6" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D7" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D8" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1343,7 +1341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1357,7 +1355,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1371,7 +1369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1385,7 +1383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1399,7 +1397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1413,7 +1411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1427,7 +1425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1441,7 +1439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1455,7 +1453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1469,7 +1467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1483,7 +1481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1497,7 +1495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1511,7 +1509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1525,7 +1523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1539,7 +1537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1553,7 +1551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1567,7 +1565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1581,7 +1579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1595,7 +1593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1609,7 +1607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1623,7 +1621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1637,7 +1635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1651,7 +1649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1665,7 +1663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1679,7 +1677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1693,7 +1691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1707,7 +1705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1721,7 +1719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1735,7 +1733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1749,7 +1747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1763,7 +1761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1777,7 +1775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1791,7 +1789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1805,7 +1803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1819,7 +1817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1833,7 +1831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1847,7 +1845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1861,7 +1859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1875,7 +1873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1889,7 +1887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1903,7 +1901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1917,7 +1915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1931,7 +1929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1945,7 +1943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1959,7 +1957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1973,7 +1971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1987,7 +1985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2001,7 +1999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2015,7 +2013,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2029,7 +2027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2043,7 +2041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2057,7 +2055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2071,7 +2069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2085,7 +2083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2099,7 +2097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2113,7 +2111,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2127,7 +2125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2141,7 +2139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2155,7 +2153,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2169,7 +2167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2183,7 +2181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2197,7 +2195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2211,7 +2209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2225,7 +2223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2239,7 +2237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2253,7 +2251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2267,7 +2265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2281,7 +2279,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2295,7 +2293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2309,7 +2307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2323,7 +2321,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2337,7 +2335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2351,7 +2349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2365,7 +2363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2379,7 +2377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2393,7 +2391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2407,7 +2405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2421,7 +2419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2435,7 +2433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2449,7 +2447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2463,7 +2461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2477,7 +2475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2491,7 +2489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2505,7 +2503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2519,7 +2517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2533,7 +2531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2547,7 +2545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2561,7 +2559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2575,7 +2573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2589,7 +2587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2603,7 +2601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2617,7 +2615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2631,7 +2629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2645,7 +2643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2659,7 +2657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2673,7 +2671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2687,7 +2685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2701,7 +2699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2715,7 +2713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2729,7 +2727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2743,7 +2741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2757,7 +2755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2771,7 +2769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2785,7 +2783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2799,7 +2797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2813,7 +2811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2827,7 +2825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2841,7 +2839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2855,7 +2853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2869,7 +2867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2883,7 +2881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2897,7 +2895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2911,7 +2909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2925,7 +2923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2939,7 +2937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2953,7 +2951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2967,7 +2965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2981,7 +2979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -2995,7 +2993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3009,7 +3007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3023,7 +3021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3044,20 +3042,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3068,7 +3066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -3079,7 +3077,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -3090,7 +3088,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>260</v>
       </c>
@@ -3098,10 +3096,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>260</v>
       </c>
@@ -3109,10 +3107,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>260</v>
       </c>
@@ -3120,10 +3118,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>260</v>
       </c>
@@ -3131,10 +3129,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>260</v>
       </c>
@@ -3142,10 +3140,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>261</v>
       </c>
@@ -3153,10 +3151,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>261</v>
       </c>
@@ -3164,10 +3162,10 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>261</v>
       </c>
@@ -3175,10 +3173,10 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>261</v>
       </c>
@@ -3186,10 +3184,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>261</v>
       </c>
@@ -3197,186 +3195,186 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
       <c r="C19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>273</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B21">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B26">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B27">
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B28">
         <v>7</v>
       </c>
       <c r="C28" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>280</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>263</v>
       </c>
       <c r="B29">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>10</v>
       </c>
@@ -3387,7 +3385,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>10</v>
       </c>

</xml_diff>